<commit_message>
Arrumando excel e site
Renomeando arquivos, arrumando categorias no excel e implementando as,
no site
</commit_message>
<xml_diff>
--- a/Clasificando projetos.xlsx
+++ b/Clasificando projetos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chend\Desktop\Insper\2º Semestre 2C\Co-design de aplicativos\Projeto 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chend\Documents\GitHub\Projeto-1-Co-design-de-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,27 +101,9 @@
     <t>Análise exploratória</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
     <t>Construção</t>
   </si>
   <si>
-    <t>Construção pura</t>
-  </si>
-  <si>
-    <t>Construção com software</t>
-  </si>
-  <si>
-    <t>Apresentação</t>
-  </si>
-  <si>
-    <t>Produção textual</t>
-  </si>
-  <si>
-    <t>Teoria</t>
-  </si>
-  <si>
     <t>Acionamento PWM com eletrônica analógica ou filtro</t>
   </si>
   <si>
@@ -129,6 +111,24 @@
   </si>
   <si>
     <t>Experimentação e testes em laboratório</t>
+  </si>
+  <si>
+    <t>Produções textuais</t>
+  </si>
+  <si>
+    <t>Apresentações</t>
+  </si>
+  <si>
+    <t>Projetos teóricos</t>
+  </si>
+  <si>
+    <t>Construções puras</t>
+  </si>
+  <si>
+    <t>Construções com softwares</t>
+  </si>
+  <si>
+    <t>Projetos envolvendo softwares</t>
   </si>
 </sst>
 </file>
@@ -286,34 +286,34 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,171 +638,171 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="19.7109375" style="4"/>
-    <col min="6" max="12" width="15" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="19.7109375" style="4"/>
+    <col min="1" max="5" width="19.7109375" style="1"/>
+    <col min="6" max="12" width="15" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="19.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>